<commit_message>
feat(excel/operation): import and export
</commit_message>
<xml_diff>
--- a/src/api/media/excel/export_org_tmpl.xlsx
+++ b/src/api/media/excel/export_org_tmpl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CanwayProject\bkuser_dev\bk-user\src\saas\media\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wklken/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4F696D-76DC-4318-9165-414CD0C4490C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F13CB3-9980-F849-8D72-D32D8764BC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="500" windowWidth="37400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_info" sheetId="1" r:id="rId1"/>
@@ -44,10 +44,6 @@
   </si>
   <si>
     <t>全名</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>在职状态</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -125,15 +121,17 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>在职状态</t>
+  </si>
+  <si>
     <t>账号过期时间</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -188,6 +186,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,7 +216,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -227,9 +232,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -248,9 +250,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -590,373 +604,373 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="9" customWidth="1"/>
     <col min="7" max="8" width="28.6640625" style="4" customWidth="1"/>
     <col min="9" max="9" width="22" style="4" customWidth="1"/>
-    <col min="10" max="10" width="39.1640625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="39.1640625" style="9" customWidth="1"/>
     <col min="11" max="11" width="17" style="4" customWidth="1"/>
     <col min="12" max="12" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="251" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+    <row r="1" spans="1:13" ht="251" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="33.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>10</v>
+      <c r="L2" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:13">
+      <c r="A3" s="11"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:13">
+      <c r="A4" s="11"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:13">
+      <c r="A5" s="11"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+    <row r="6" spans="1:13">
+      <c r="A6" s="11"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+    <row r="7" spans="1:13">
+      <c r="A7" s="11"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:13">
+      <c r="A8" s="11"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:13">
+      <c r="A9" s="11"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:13">
+      <c r="A10" s="11"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:13">
+      <c r="A11" s="11"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+    <row r="12" spans="1:13">
+      <c r="A12" s="11"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+    <row r="13" spans="1:13">
+      <c r="A13" s="11"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+    <row r="14" spans="1:13">
+      <c r="A14" s="11"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+    <row r="15" spans="1:13">
+      <c r="A15" s="11"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+    <row r="16" spans="1:13">
+      <c r="A16" s="11"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+    <row r="17" spans="1:10">
+      <c r="A17" s="11"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+    <row r="18" spans="1:10">
+      <c r="A18" s="11"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+    <row r="19" spans="1:10">
+      <c r="A19" s="11"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+    <row r="20" spans="1:10">
+      <c r="A20" s="11"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+    <row r="21" spans="1:10">
+      <c r="A21" s="11"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+    <row r="22" spans="1:10">
+      <c r="A22" s="11"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+    <row r="23" spans="1:10">
+      <c r="A23" s="11"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="D23" s="11"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+    <row r="24" spans="1:10">
+      <c r="A24" s="11"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+    <row r="25" spans="1:10">
+      <c r="A25" s="11"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+    <row r="26" spans="1:10">
+      <c r="A26" s="11"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
+    <row r="27" spans="1:10">
+      <c r="A27" s="11"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="11"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
+    <row r="28" spans="1:10">
+      <c r="A28" s="11"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+      <c r="D28" s="11"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+    <row r="29" spans="1:10">
+      <c r="A29" s="11"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="D29" s="11"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+    <row r="30" spans="1:10">
+      <c r="A30" s="11"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
+    <row r="31" spans="1:10">
+      <c r="A31" s="11"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+    <row r="32" spans="1:10">
+      <c r="A32" s="11"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+    <row r="33" spans="1:10">
+      <c r="A33" s="11"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
+    <row r="34" spans="1:10">
+      <c r="A34" s="11"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+    <row r="35" spans="1:10">
+      <c r="A35" s="11"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
+      <c r="D35" s="11"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="J35" s="4"/>

</xml_diff>

<commit_message>
feat(api/web): add audit log for create/update/delete (#710)
* feat(api/web): add audit log for create/update/delete
* fix(local/import): report fail record during import from excel
* fix(saas/bugs): fix bugs in the testing
* fix(api/ldap): address from ldap://localhost:389 to ldap://127.0.0.1:389
* feat(audit/login): export
* docs(api/v2): comment the used api urls
* feat(excel/operation): import and export
* fix(profile/patch): update lost the extras field
* fix(audit/log): decorator make the drf fail
</commit_message>
<xml_diff>
--- a/src/api/media/excel/export_org_tmpl.xlsx
+++ b/src/api/media/excel/export_org_tmpl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CanwayProject\bkuser_dev\bk-user\src\saas\media\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wklken/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4F696D-76DC-4318-9165-414CD0C4490C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F13CB3-9980-F849-8D72-D32D8764BC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="500" windowWidth="37400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_info" sheetId="1" r:id="rId1"/>
@@ -44,10 +44,6 @@
   </si>
   <si>
     <t>全名</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>在职状态</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -125,15 +121,17 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>在职状态</t>
+  </si>
+  <si>
     <t>账号过期时间</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -188,6 +186,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,7 +216,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -227,9 +232,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -248,9 +250,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -590,373 +604,373 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="9" customWidth="1"/>
     <col min="7" max="8" width="28.6640625" style="4" customWidth="1"/>
     <col min="9" max="9" width="22" style="4" customWidth="1"/>
-    <col min="10" max="10" width="39.1640625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="39.1640625" style="9" customWidth="1"/>
     <col min="11" max="11" width="17" style="4" customWidth="1"/>
     <col min="12" max="12" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="251" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+    <row r="1" spans="1:13" ht="251" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="33.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>10</v>
+      <c r="L2" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:13">
+      <c r="A3" s="11"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:13">
+      <c r="A4" s="11"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:13">
+      <c r="A5" s="11"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+    <row r="6" spans="1:13">
+      <c r="A6" s="11"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+    <row r="7" spans="1:13">
+      <c r="A7" s="11"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:13">
+      <c r="A8" s="11"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:13">
+      <c r="A9" s="11"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:13">
+      <c r="A10" s="11"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:13">
+      <c r="A11" s="11"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+    <row r="12" spans="1:13">
+      <c r="A12" s="11"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+    <row r="13" spans="1:13">
+      <c r="A13" s="11"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+    <row r="14" spans="1:13">
+      <c r="A14" s="11"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+    <row r="15" spans="1:13">
+      <c r="A15" s="11"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+    <row r="16" spans="1:13">
+      <c r="A16" s="11"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+    <row r="17" spans="1:10">
+      <c r="A17" s="11"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+    <row r="18" spans="1:10">
+      <c r="A18" s="11"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+    <row r="19" spans="1:10">
+      <c r="A19" s="11"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+    <row r="20" spans="1:10">
+      <c r="A20" s="11"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+    <row r="21" spans="1:10">
+      <c r="A21" s="11"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+    <row r="22" spans="1:10">
+      <c r="A22" s="11"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+    <row r="23" spans="1:10">
+      <c r="A23" s="11"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="D23" s="11"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+    <row r="24" spans="1:10">
+      <c r="A24" s="11"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+    <row r="25" spans="1:10">
+      <c r="A25" s="11"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+    <row r="26" spans="1:10">
+      <c r="A26" s="11"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
+    <row r="27" spans="1:10">
+      <c r="A27" s="11"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="11"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
+    <row r="28" spans="1:10">
+      <c r="A28" s="11"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+      <c r="D28" s="11"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+    <row r="29" spans="1:10">
+      <c r="A29" s="11"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="D29" s="11"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+    <row r="30" spans="1:10">
+      <c r="A30" s="11"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
+    <row r="31" spans="1:10">
+      <c r="A31" s="11"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+    <row r="32" spans="1:10">
+      <c r="A32" s="11"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+    <row r="33" spans="1:10">
+      <c r="A33" s="11"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
+    <row r="34" spans="1:10">
+      <c r="A34" s="11"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+    <row r="35" spans="1:10">
+      <c r="A35" s="11"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
+      <c r="D35" s="11"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="J35" s="4"/>

</xml_diff>

<commit_message>
Fix i18n trans (#982)
* fix: login error when account is staff out

* fix: logo error when create user

* fix: expired account is still invalid after adjusting the validity period

* feat: change display name of account_expiration_date field

* feat(api i18n): improve translation and support to translate when set bk_language header

* feat(login i18n): call usermgr api support transparent language

* fix(api i18n): impove translation
</commit_message>
<xml_diff>
--- a/src/api/media/excel/export_org_tmpl.xlsx
+++ b/src/api/media/excel/export_org_tmpl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wklken/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiananzhang/workspace/devcloud_file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F13CB3-9980-F849-8D72-D32D8764BC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5E846F-F60C-9940-A9F4-B16BD1ADDBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="37400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_info" sheetId="1" r:id="rId1"/>
@@ -47,17 +47,36 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>上级</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>账户状态</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在职状态</t>
+  </si>
+  <si>
+    <t>账号过期时间</t>
+  </si>
+  <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>填写须知：
     1、表头代表用户字段，每行数据代表一个用户。</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="18"/>
+        <sz val="16"/>
         <color rgb="FFFF0000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>用户名字段不能增删或者修改，需要和用户管理中保持完全一致</t>
@@ -65,9 +84,8 @@
     <r>
       <rPr>
         <b/>
-        <sz val="18"/>
+        <sz val="16"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>。
@@ -81,10 +99,9 @@
     <r>
       <rPr>
         <b/>
-        <sz val="18"/>
+        <sz val="16"/>
         <color rgb="FFFF0000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>选项值，</t>
@@ -92,10 +109,9 @@
     <r>
       <rPr>
         <b/>
-        <sz val="18"/>
+        <sz val="16"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>多选请以英文逗号（,）分隔</t>
@@ -103,35 +119,27 @@
     <r>
       <rPr>
         <b/>
-        <sz val="18"/>
+        <sz val="16"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>。</t>
+      <t>。
+Instructions for filling out:
+    1. The table header represents user fields, and each row of data represents a user. The username field cannot be added, deleted or modified, and must be exactly the same as in the user management.å
+    2. Fields with red names are required fields, while those with black names are optional.
+    3. Username: Unique identifier (username) for the user, consisting of 1-32 letters, numbers, dots (.), hyphens (-), or underscores (_). If usernames are the same they will be overwritten by updates.
+    4. Organization: Separate superior and subordinate organizations using '/', starting from the highest level organization; separate multiple organizations using commas (,), with individual organization names not exceeding 32 characters in length. If an organizational link does not exist it will be automatically created.
+    5. Mobile phone number: Default area code is +86 (CN) for China region; other regions need to add country/region codes in this format "+85259****24".
+    6. Direct supervisor: Fill in the superior's username (username); separate multiple superiors using commas (,).
+    7. Custom fields: For enumerated values please fill in option values; use commas to separate multiple selections.</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>上级</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>账户状态</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>在职状态</t>
-  </si>
-  <si>
-    <t>账号过期时间</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -171,26 +179,30 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FFFF0000"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="1"/>
+      <sz val="16"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -217,7 +229,7 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -227,9 +239,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -247,20 +256,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,376 +616,375 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="9" customWidth="1"/>
-    <col min="7" max="8" width="28.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="22" style="4" customWidth="1"/>
-    <col min="10" max="10" width="39.1640625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="17" style="4" customWidth="1"/>
-    <col min="12" max="12" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="8" customWidth="1"/>
+    <col min="7" max="8" width="28.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22" style="3" customWidth="1"/>
+    <col min="10" max="10" width="39.1640625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="17" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="251" customHeight="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13" ht="409" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>9</v>
-      </c>
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="11"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="11"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="11"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="11"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="11"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="11"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="11"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="11"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="11"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="11"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="11"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="11"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="11"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="11"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="11"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="11"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="11"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="11"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="11"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="11"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="J22" s="3"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="11"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="11"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="J24" s="4"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="11"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="11"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="J26" s="3"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="11"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="J27" s="3"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="11"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="J28" s="3"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="11"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="11"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="11"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="J31" s="3"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="11"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="J32" s="4"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="J32" s="3"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="11"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="J33" s="4"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="J33" s="3"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="11"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="J34" s="3"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="11"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="J35" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>